<commit_message>
New features on notebook
First cell in feature selection
</commit_message>
<xml_diff>
--- a/techscape-ecommerce/new_variables.xlsx
+++ b/techscape-ecommerce/new_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b08d5fd33581ba77/OneDrive Docs/Documents/Masters/Machine Learning/kaggle_ml_35/techscape-ecommerce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E60C0B2-2909-4465-95E4-73C59B85A454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{0E60C0B2-2909-4465-95E4-73C59B85A454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3F1A136-A947-4AEC-9F5C-EAB0887CAFBD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8FD2E862-170C-4089-AC14-7F38B0A467A9}"/>
+    <workbookView xWindow="3384" yWindow="3276" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{8FD2E862-170C-4089-AC14-7F38B0A467A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="254">
   <si>
     <t>chi-squared</t>
   </si>
@@ -756,6 +756,48 @@
   </si>
   <si>
     <t>Metric_1model</t>
+  </si>
+  <si>
+    <t>2 methods</t>
+  </si>
+  <si>
+    <t>3 methods</t>
+  </si>
+  <si>
+    <t>4 methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountMng_Pages', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_duration_FAQ', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_Product_Duration', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_Pages', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_BounceRate', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_ExitRate', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_PageValue', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_duration_product', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoogleAnalytics_BounceRate', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoogleAnalytics_ExitRate', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoogleAnalytics_PageValue', </t>
   </si>
 </sst>
 </file>
@@ -789,7 +831,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -820,6 +862,24 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE96584"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -846,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -875,12 +935,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE96584"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2732,22 +2800,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E93458F-2044-4C41-93A8-53902F096797}">
-  <dimension ref="B4:N76"/>
+  <dimension ref="B3:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="J34" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="11" max="13" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" customWidth="1"/>
+    <col min="12" max="13" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>115</v>
       </c>
@@ -2764,7 +2835,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>90</v>
       </c>
@@ -2796,7 +2867,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>95</v>
       </c>
@@ -2817,20 +2888,20 @@
         <f>SUM(C6:F6)</f>
         <v>4</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>96</v>
       </c>
@@ -2842,20 +2913,20 @@
         <f t="shared" ref="G7:G70" si="0">SUM(C7:F7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -2870,20 +2941,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="18" t="s">
         <v>100</v>
       </c>
       <c r="N8" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>98</v>
       </c>
@@ -2898,7 +2969,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="18" t="s">
         <v>99</v>
       </c>
       <c r="L9" s="13" t="s">
@@ -2907,11 +2978,11 @@
       <c r="M9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -2932,7 +3003,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="18" t="s">
         <v>100</v>
       </c>
       <c r="L10" s="14" t="s">
@@ -2945,7 +3016,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>100</v>
       </c>
@@ -2979,7 +3050,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>101</v>
       </c>
@@ -3003,14 +3074,14 @@
       <c r="K12" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>102</v>
       </c>
@@ -3034,14 +3105,14 @@
       <c r="K13" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>103</v>
       </c>
@@ -3062,7 +3133,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="16" t="s">
         <v>104</v>
       </c>
       <c r="L14" s="14" t="s">
@@ -3072,7 +3143,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>104</v>
       </c>
@@ -3093,17 +3164,17 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="16" t="s">
         <v>108</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>105</v>
       </c>
@@ -3124,11 +3195,11 @@
       <c r="K16" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>106</v>
       </c>
@@ -3146,14 +3217,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="K17" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>107</v>
       </c>
@@ -3168,14 +3239,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="16" t="s">
         <v>108</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>108</v>
       </c>
@@ -3193,14 +3264,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="17" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>109</v>
       </c>
@@ -3212,14 +3283,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="18" t="s">
         <v>111</v>
       </c>
       <c r="L20" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>110</v>
       </c>
@@ -3234,11 +3305,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>111</v>
       </c>
@@ -3263,7 +3334,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>112</v>
       </c>
@@ -3285,7 +3356,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>113</v>
       </c>
@@ -3307,7 +3378,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>114</v>
       </c>
@@ -3329,7 +3400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>223</v>
       </c>
@@ -3350,14 +3421,32 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>240</v>
+      </c>
+      <c r="M26" t="s">
+        <v>241</v>
+      </c>
+      <c r="N26" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="G27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L27" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="M27" t="s">
+        <v>95</v>
+      </c>
+      <c r="N27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>116</v>
       </c>
@@ -3376,14 +3465,17 @@
       <c r="G28" t="s">
         <v>238</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L28" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="M28" t="s">
+        <v>101</v>
+      </c>
+      <c r="N28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>117</v>
       </c>
@@ -3395,14 +3487,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L29" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="M29" t="s">
+        <v>102</v>
+      </c>
+      <c r="N29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>118</v>
       </c>
@@ -3414,12 +3509,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K30" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L30" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="M30" t="s">
+        <v>103</v>
+      </c>
+      <c r="N30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>119</v>
       </c>
@@ -3431,11 +3531,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L31" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M31" t="s">
+        <v>114</v>
+      </c>
+      <c r="N31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>120</v>
       </c>
@@ -3447,11 +3553,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="M32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>121</v>
       </c>
@@ -3463,11 +3572,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="M33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>122</v>
       </c>
@@ -3479,11 +3591,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K34" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="M34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>123</v>
       </c>
@@ -3495,11 +3610,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>124</v>
       </c>
@@ -3511,11 +3626,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>125</v>
       </c>
@@ -3527,11 +3642,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>126</v>
       </c>
@@ -3544,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>127</v>
       </c>
@@ -3557,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>128</v>
       </c>
@@ -3570,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>129</v>
       </c>
@@ -3583,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>130</v>
       </c>
@@ -3596,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>131</v>
       </c>
@@ -3609,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>132</v>
       </c>
@@ -3622,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>133</v>
       </c>
@@ -3635,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>134</v>
       </c>
@@ -3648,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>135</v>
       </c>
@@ -3660,8 +3775,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K47" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>136</v>
       </c>
@@ -3673,8 +3794,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K48" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="L48" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>224</v>
       </c>
@@ -3686,8 +3813,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K49" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>137</v>
       </c>
@@ -3699,8 +3830,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K50" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="12" t="s">
         <v>225</v>
       </c>
@@ -3712,8 +3846,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K51" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>138</v>
       </c>
@@ -3725,8 +3862,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K52" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>139</v>
       </c>
@@ -3738,8 +3878,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K53" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>140</v>
       </c>
@@ -3751,8 +3894,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K54" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>141</v>
       </c>
@@ -3764,8 +3910,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K55" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>142</v>
       </c>
@@ -3777,8 +3926,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K56" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>143</v>
       </c>
@@ -3791,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>144</v>
       </c>
@@ -3804,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>145</v>
       </c>
@@ -3817,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>146</v>
       </c>
@@ -3830,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>147</v>
       </c>
@@ -3843,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>148</v>
       </c>
@@ -3856,7 +4008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>149</v>
       </c>
@@ -3869,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>150</v>
       </c>
@@ -4042,6 +4194,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N27:N31">
+    <sortCondition ref="N27:N31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>